<commit_message>
minor changes to columns' name
</commit_message>
<xml_diff>
--- a/results/motif_representation_table.xlsx
+++ b/results/motif_representation_table.xlsx
@@ -1,15 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="GLiFmDzCpJhZDe/0iyxHYZwqKuITyxQySLE83+5xbvE="/>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -18,594 +22,610 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2422" uniqueCount="189">
   <si>
-    <t>graph_name</t>
-  </si>
-  <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t>S2</t>
-  </si>
-  <si>
-    <t>S3</t>
-  </si>
-  <si>
-    <t>S4</t>
-  </si>
-  <si>
-    <t>S5</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>D4</t>
-  </si>
-  <si>
-    <t>D5</t>
-  </si>
-  <si>
-    <t>D6</t>
-  </si>
-  <si>
-    <t>D7</t>
-  </si>
-  <si>
-    <t>D8</t>
-  </si>
-  <si>
-    <t>Lower Chesapeake Bay</t>
-  </si>
-  <si>
-    <t>🔺</t>
-  </si>
-  <si>
-    <t>⬇</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Middle Chesapeake Bay</t>
-  </si>
-  <si>
-    <t>Upper Chesapeake Bay</t>
-  </si>
-  <si>
-    <t>Chesapeake Bay Mesohaline</t>
-  </si>
-  <si>
-    <t>Charca de Maspalomas</t>
-  </si>
-  <si>
-    <t>Mondego Estuary - Zostrea site</t>
-  </si>
-  <si>
-    <t>Narragansett Bay Model</t>
-  </si>
-  <si>
-    <t>St. Marks River (Florida)</t>
-  </si>
-  <si>
-    <t>Aegean Sea (2003)</t>
-  </si>
-  <si>
-    <t>Albatross Bay (1986)</t>
-  </si>
-  <si>
-    <t>Aleutian Islands (1963)</t>
-  </si>
-  <si>
-    <t>Alto Golfo de California (0)</t>
-  </si>
-  <si>
-    <t>Antarctic (1970)</t>
-  </si>
-  <si>
-    <t>Australia North West Shelf (1986)</t>
-  </si>
-  <si>
-    <t>Azores (1997)</t>
-  </si>
-  <si>
-    <t>Azores archipelago (1997)</t>
-  </si>
-  <si>
-    <t>Baie de Seine (2000)</t>
-  </si>
-  <si>
-    <t>Bay of Biscay (1970)</t>
-  </si>
-  <si>
-    <t>Bay of Biscay (1980)</t>
-  </si>
-  <si>
-    <t>Bay of Biscay (1994)</t>
-  </si>
-  <si>
-    <t>Bay of Biscay (1998)</t>
-  </si>
-  <si>
-    <t>Bay of Biscay (2013)</t>
-  </si>
-  <si>
-    <t>Bolinao Coral Reef (1980)</t>
-  </si>
-  <si>
-    <t>Calvi Bay (1998)</t>
-  </si>
-  <si>
-    <t>Cap de Creus MPA - whole (2008)</t>
-  </si>
-  <si>
-    <t>Cape Verde (1981)</t>
-  </si>
-  <si>
-    <t>Celtic Sea-Biscay (1980)</t>
-  </si>
-  <si>
-    <t>Celtic Sea-Biscay (2012)</t>
-  </si>
-  <si>
-    <t>Celtic Sea (1980)</t>
-  </si>
-  <si>
-    <t>Celtic Sea (1985)</t>
-  </si>
-  <si>
-    <t>Celtic Sea (2013)</t>
-  </si>
-  <si>
-    <t>Central Atlantic (1950)</t>
-  </si>
-  <si>
-    <t>Central Atlantic (1990)</t>
-  </si>
-  <si>
-    <t>Central Baltic Sea (1974)</t>
-  </si>
-  <si>
-    <t>Central Gulf of California (1978)</t>
-  </si>
-  <si>
-    <t>Cerbère-Banyuls MPA (2013)</t>
-  </si>
-  <si>
-    <t>Chesapeake (1950)</t>
-  </si>
-  <si>
-    <t>Contemporary Alosine (2000)</t>
-  </si>
-  <si>
-    <t>Cypress Dry Season</t>
-  </si>
-  <si>
-    <t>Cypress Wet Season</t>
-  </si>
-  <si>
-    <t>Deep Western Mediterranean sea (2009)</t>
-  </si>
-  <si>
-    <t>Denmark, Faroe Islands (1997)</t>
-  </si>
-  <si>
-    <t>East Bass Strait (1994)</t>
-  </si>
-  <si>
-    <t>Eastern Corsican Coast (2012)</t>
-  </si>
-  <si>
-    <t>Falkland Islands (1990)</t>
-  </si>
-  <si>
-    <t>Galapagos (2006)</t>
-  </si>
-  <si>
-    <t>Galapagos, Floreana rocky reef (2000)</t>
-  </si>
-  <si>
-    <t>Greenland, West Coast (1997)</t>
-  </si>
-  <si>
-    <t>Guinea (1985)</t>
-  </si>
-  <si>
-    <t>Guinea (1998)</t>
-  </si>
-  <si>
-    <t>Guinea  (2004)</t>
-  </si>
-  <si>
-    <t>Gulf of California (1990)</t>
-  </si>
-  <si>
-    <t>Gulf of Carpentaria (1990)</t>
-  </si>
-  <si>
-    <t>Gulf of Gabes (2000)</t>
-  </si>
-  <si>
-    <t>Gulf of Thailande (1963)</t>
-  </si>
-  <si>
-    <t>Hudson Bay (1970)</t>
-  </si>
-  <si>
-    <t>Humboldt Current (1995)</t>
-  </si>
-  <si>
-    <t>Iceland (1950)</t>
-  </si>
-  <si>
-    <t>Icelandic shelf (1997)</t>
-  </si>
-  <si>
-    <t>Independence Bay (1996)</t>
-  </si>
-  <si>
-    <t>Irish Sea (1973)</t>
-  </si>
-  <si>
-    <t>Jalisco and Colima Coast (1995)</t>
-  </si>
-  <si>
-    <t>Jurien Bay (2007)</t>
-  </si>
-  <si>
-    <t>Kaloko Honokohau (2005)</t>
-  </si>
-  <si>
-    <t>Lesser Antilles (2001)</t>
-  </si>
-  <si>
-    <t>Little Rock Lake, Wisconsin</t>
-  </si>
-  <si>
-    <t>Looe Key National Marine Sanctuary (1980)</t>
-  </si>
-  <si>
-    <t>Malangen Fjord (2017)</t>
-  </si>
-  <si>
-    <t>Tasek Bera swamp, Malaysia</t>
-  </si>
-  <si>
-    <t>Mauritania (1987)</t>
-  </si>
-  <si>
-    <t>Mauritania (1998)</t>
-  </si>
-  <si>
-    <t>Mauritanie  (1991)</t>
-  </si>
-  <si>
-    <t>Medes Island MPA (2000)</t>
-  </si>
-  <si>
-    <t>Morocco (1985)</t>
-  </si>
-  <si>
-    <t>Mount St Michel Bay (2003)</t>
-  </si>
-  <si>
-    <t>Ningaloo (2007)</t>
-  </si>
-  <si>
-    <t>North Atlantic (1950)</t>
-  </si>
-  <si>
-    <t>North Atlantic (1997)</t>
-  </si>
-  <si>
-    <t>North Benguela (1600)</t>
-  </si>
-  <si>
-    <t>North Benguela (1900)</t>
-  </si>
-  <si>
-    <t>North Benguela (1967)</t>
-  </si>
-  <si>
-    <t>North Benguela (1990)</t>
-  </si>
-  <si>
-    <t>North Sea (1974)</t>
-  </si>
-  <si>
-    <t>North Sea (1981)</t>
-  </si>
-  <si>
-    <t>North South of China Sea (1970)</t>
-  </si>
-  <si>
-    <t>Northern Benguela (1956)</t>
-  </si>
-  <si>
-    <t>Northern British Columbia (1950)</t>
-  </si>
-  <si>
-    <t>Northern British Columbia (2000)</t>
-  </si>
-  <si>
-    <t>Northern Californian Current (1960)</t>
-  </si>
-  <si>
-    <t>Northern Californian Current (1990)</t>
-  </si>
-  <si>
-    <t>Northern Gulf of Mexico (2005)</t>
-  </si>
-  <si>
-    <t>Northern Gulf of St Lawrence (1990)</t>
-  </si>
-  <si>
-    <t>Northern Gulf St Lawrence (1985)</t>
-  </si>
-  <si>
-    <t>Northern Humboldt Current (1997)</t>
-  </si>
-  <si>
-    <t>Port Cros (1998)</t>
-  </si>
-  <si>
-    <t>Port Phillip Bay (1994)</t>
-  </si>
-  <si>
-    <t>Prince William Sound (1994)</t>
-  </si>
-  <si>
-    <t>Raja Ampat (1990)</t>
-  </si>
-  <si>
-    <t>Raja Ampat (2005)</t>
-  </si>
-  <si>
-    <t>Restored Alosine Biomass (2000)</t>
-  </si>
-  <si>
-    <t>Rocky shore, Monterey Bay, California</t>
-  </si>
-  <si>
-    <t>Salt meadow, New Zealand</t>
-  </si>
-  <si>
-    <t>Sand beach, South Africa</t>
-  </si>
-  <si>
-    <t>Sechura Bay (1996)</t>
-  </si>
-  <si>
-    <t>Shallow sublittoral, Cape Ann, Massachusetts</t>
-  </si>
-  <si>
-    <t>Sierra Leone (1964)</t>
-  </si>
-  <si>
-    <t>Sierra Leone 1978 (1978)</t>
-  </si>
-  <si>
-    <t>Sierra Leone (1990)</t>
-  </si>
-  <si>
-    <t>Sinaloa sur MEXICO (1994)</t>
-  </si>
-  <si>
-    <t>Sirinhaém River (2013)</t>
-  </si>
-  <si>
-    <t>Sonda_Campeche_Act (1988)</t>
-  </si>
-  <si>
-    <t>South Benguela (1600)</t>
-  </si>
-  <si>
-    <t>South Benguela (1900)</t>
-  </si>
-  <si>
-    <t>South Benguela (1978)</t>
-  </si>
-  <si>
-    <t>South East Alaska (1963)</t>
-  </si>
-  <si>
-    <t>South of Benguela (1960)</t>
-  </si>
-  <si>
-    <t>South Shetlands (1990)</t>
-  </si>
-  <si>
-    <t>South western Gulf of Mexico (1970)</t>
-  </si>
-  <si>
-    <t>Sørfjord (1993)</t>
-  </si>
-  <si>
-    <t>Tasmanian Seamounts Marine Reserve (1992)</t>
-  </si>
-  <si>
-    <t>Terminos Lagoon (1980)</t>
-  </si>
-  <si>
-    <t>Thermaikos Gulf (1998)</t>
-  </si>
-  <si>
-    <t>Tropical plankton community, Pacific</t>
-  </si>
-  <si>
-    <t>USA, Mid Atlantic Bight (1995)</t>
-  </si>
-  <si>
-    <t>USA, South Atlantic Continental Shelf (1995)</t>
-  </si>
-  <si>
-    <t>Virgin Islands (1960)</t>
-  </si>
-  <si>
-    <t>West Baffin Bay, Coastal and Shelf (2016)</t>
-  </si>
-  <si>
-    <t>West Florida Shelf Historic Model (1950)</t>
-  </si>
-  <si>
-    <t>West Scotland (2000)</t>
-  </si>
-  <si>
-    <t>Western Antarctic Peninsula (1996)</t>
-  </si>
-  <si>
-    <t>Western Channel (1973)</t>
-  </si>
-  <si>
-    <t>Western Channel (1993)</t>
-  </si>
-  <si>
-    <t>Western Tropical Pacific Ocean (1990)</t>
-  </si>
-  <si>
-    <t>Yucatan (1987)</t>
-  </si>
-  <si>
-    <t>Crystal River Creek - Control</t>
-  </si>
-  <si>
-    <t>Crystal River Creek - Delta Temp</t>
-  </si>
-  <si>
-    <t>Lake Michigan</t>
-  </si>
-  <si>
-    <t>Apalachicola Bay (2000)</t>
-  </si>
-  <si>
-    <t>Arctic seas</t>
-  </si>
-  <si>
-    <t>Bamboung (2003)</t>
-  </si>
-  <si>
-    <t>Bamboung (2006)</t>
-  </si>
-  <si>
-    <t>Barnegat Bay (1981)</t>
-  </si>
-  <si>
-    <t>Barra Del Chuy (1992)</t>
-  </si>
-  <si>
-    <t>Florida Bay - dry season</t>
-  </si>
-  <si>
-    <t>Florida Bay - wet season</t>
-  </si>
-  <si>
-    <t>British Columbia coast (1950)</t>
-  </si>
-  <si>
-    <t>Central Chile (1998)</t>
-  </si>
-  <si>
-    <t>Lake Paajarvi, littoral zone, Finland</t>
-  </si>
-  <si>
-    <t>Lake Pyhajarvi, littoral zone, Finland</t>
-  </si>
-  <si>
-    <t>Florida Bay (2006)</t>
-  </si>
-  <si>
-    <t>Everglades Graminoids</t>
-  </si>
-  <si>
-    <t>Gulf of Mexico (1950)</t>
-  </si>
-  <si>
-    <t>Huizache-Caimanero (1984)</t>
-  </si>
-  <si>
-    <t>Mangrove Estuary - Dry Season</t>
-  </si>
-  <si>
-    <t>Mangrove Estuary - Wet Season</t>
-  </si>
-  <si>
-    <t>North East Pacific (1950)</t>
-  </si>
-  <si>
-    <t>Paraná River Floodplain (1992)</t>
-  </si>
-  <si>
-    <t>Peru (1953)</t>
-  </si>
-  <si>
-    <t>Peru (1960)</t>
-  </si>
-  <si>
-    <t>Peru (1973)</t>
-  </si>
-  <si>
-    <t>Ria-Lake Tapajos (2013)</t>
-  </si>
-  <si>
-    <t>Santa Pola Bay (2001)</t>
-  </si>
-  <si>
-    <t>Sítios Novos reservoir (2011)</t>
-  </si>
-  <si>
-    <t>Sri Lanka (2000)</t>
-  </si>
-  <si>
-    <t>Strait of Georgia (1950)</t>
-  </si>
-  <si>
-    <t>Swamp, south Florida</t>
-  </si>
-  <si>
-    <t>Tampa Bay (1950)</t>
+    <t xml:space="preserve">Network</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lower Chesapeake Bay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🔺</t>
+  </si>
+  <si>
+    <t xml:space="preserve">⬇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Middle Chesapeake Bay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upper Chesapeake Bay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chesapeake Bay Mesohaline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charca de Maspalomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mondego Estuary - Zostrea site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Narragansett Bay Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">St. Marks River (Florida)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aegean Sea (2003)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Albatross Bay (1986)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aleutian Islands (1963)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alto Golfo de California (0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antarctic (1970)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Australia North West Shelf (1986)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Azores (1997)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Azores archipelago (1997)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baie de Seine (2000)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bay of Biscay (1970)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bay of Biscay (1980)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bay of Biscay (1994)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bay of Biscay (1998)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bay of Biscay (2013)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bolinao Coral Reef (1980)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calvi Bay (1998)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cap de Creus MPA - whole (2008)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cape Verde (1981)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Celtic Sea-Biscay (1980)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Celtic Sea-Biscay (2012)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Celtic Sea (1980)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Celtic Sea (1985)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Celtic Sea (2013)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central Atlantic (1950)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central Atlantic (1990)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central Baltic Sea (1974)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central Gulf of California (1978)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cerbère-Banyuls MPA (2013)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chesapeake (1950)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contemporary Alosine (2000)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cypress Dry Season</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cypress Wet Season</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deep Western Mediterranean sea (2009)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denmark, Faroe Islands (1997)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East Bass Strait (1994)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastern Corsican Coast (2012)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falkland Islands (1990)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Galapagos (2006)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Galapagos, Floreana rocky reef (2000)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greenland, West Coast (1997)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guinea (1985)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guinea (1998)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guinea  (2004)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of California (1990)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Carpentaria (1990)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Gabes (2000)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Thailande (1963)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hudson Bay (1970)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Humboldt Current (1995)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iceland (1950)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Icelandic shelf (1997)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Independence Bay (1996)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Irish Sea (1973)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jalisco and Colima Coast (1995)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jurien Bay (2007)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kaloko Honokohau (2005)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lesser Antilles (2001)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Little Rock Lake, Wisconsin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Looe Key National Marine Sanctuary (1980)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malangen Fjord (2017)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tasek Bera swamp, Malaysia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mauritania (1987)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mauritania (1998)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mauritanie  (1991)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medes Island MPA (2000)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morocco (1985)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mount St Michel Bay (2003)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ningaloo (2007)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Atlantic (1950)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Atlantic (1997)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Benguela (1600)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Benguela (1900)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Benguela (1967)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Benguela (1990)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Sea (1974)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Sea (1981)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North South of China Sea (1970)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Benguela (1956)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern British Columbia (1950)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern British Columbia (2000)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Californian Current (1960)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Californian Current (1990)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Gulf of Mexico (2005)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Gulf of St Lawrence (1990)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Gulf St Lawrence (1985)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Humboldt Current (1997)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Port Cros (1998)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Port Phillip Bay (1994)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prince William Sound (1994)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raja Ampat (1990)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raja Ampat (2005)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restored Alosine Biomass (2000)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rocky shore, Monterey Bay, California</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salt meadow, New Zealand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sand beach, South Africa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sechura Bay (1996)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shallow sublittoral, Cape Ann, Massachusetts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sierra Leone (1964)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sierra Leone 1978 (1978)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sierra Leone (1990)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sinaloa sur MEXICO (1994)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sirinhaém River (2013)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sonda_Campeche_Act (1988)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Benguela (1600)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Benguela (1900)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Benguela (1978)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South East Alaska (1963)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South of Benguela (1960)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Shetlands (1990)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South western Gulf of Mexico (1970)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sørfjord (1993)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tasmanian Seamounts Marine Reserve (1992)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terminos Lagoon (1980)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thermaikos Gulf (1998)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tropical plankton community, Pacific</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USA, Mid Atlantic Bight (1995)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USA, South Atlantic Continental Shelf (1995)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virgin Islands (1960)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">West Baffin Bay, Coastal and Shelf (2016)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">West Florida Shelf Historic Model (1950)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">West Scotland (2000)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Antarctic Peninsula (1996)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Channel (1973)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Channel (1993)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Tropical Pacific Ocean (1990)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yucatan (1987)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crystal River Creek - Control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crystal River Creek - Delta Temp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lake Michigan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apalachicola Bay (2000)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arctic seas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bamboung (2003)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bamboung (2006)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barnegat Bay (1981)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barra Del Chuy (1992)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Florida Bay - dry season</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Florida Bay - wet season</t>
+  </si>
+  <si>
+    <t xml:space="preserve">British Columbia coast (1950)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central Chile (1998)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lake Paajarvi, littoral zone, Finland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lake Pyhajarvi, littoral zone, Finland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Florida Bay (2006)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Everglades Graminoids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulf of Mexico (1950)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huizache-Caimanero (1984)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mangrove Estuary - Dry Season</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mangrove Estuary - Wet Season</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North East Pacific (1950)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paraná River Floodplain (1992)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peru (1953)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peru (1960)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peru (1973)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ria-Lake Tapajos (2013)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Santa Pola Bay (2001)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sítios Novos reservoir (2011)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sri Lanka (2000)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strait of Georgia (1950)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swamp, south Florida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tampa Bay (1950)</t>
   </si>
   <si>
     <t xml:space="preserve">Tagus estuary, Portugal </t>
   </si>
   <si>
-    <t>West coast of Sabah (1972)</t>
-  </si>
-  <si>
-    <t>West Florida Shelf (1985)</t>
-  </si>
-  <si>
-    <t>West scotland DeepSea (1974)</t>
-  </si>
-  <si>
-    <t>Ythan estuary, Aberdeenshire, Scotland</t>
+    <t xml:space="preserve">West coast of Sabah (1972)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">West Florida Shelf (1985)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">West scotland DeepSea (1974)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ythan estuary, Aberdeenshire, Scotland</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="General"/>
+  </numFmts>
+  <fonts count="5">
     <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
-      <color theme="1"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -613,261 +633,95 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
-  <a:themeElements>
-    <a:clrScheme name="Sheets">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="0000FF"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Sheets">
-      <a:majorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface="Calibri"/>
-        <a:cs typeface="Calibri"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface="Calibri"/>
-        <a:cs typeface="Calibri"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="40.71"/>
-    <col customWidth="1" min="2" max="26" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="8.7"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -911,7 +765,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -955,7 +809,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -999,7 +853,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -1043,7 +897,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -1087,7 +941,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -1131,7 +985,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -1175,7 +1029,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1219,7 +1073,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -1263,7 +1117,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -1307,7 +1161,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -1351,7 +1205,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -1395,7 +1249,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1439,7 +1293,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
@@ -1483,7 +1337,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
@@ -1527,7 +1381,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
@@ -1571,7 +1425,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -1615,7 +1469,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
@@ -1659,7 +1513,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
@@ -1703,7 +1557,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>35</v>
       </c>
@@ -1747,7 +1601,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -1791,7 +1645,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
@@ -1835,7 +1689,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>38</v>
       </c>
@@ -1879,7 +1733,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>39</v>
       </c>
@@ -1923,7 +1777,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>40</v>
       </c>
@@ -1967,7 +1821,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>41</v>
       </c>
@@ -2011,7 +1865,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>42</v>
       </c>
@@ -2055,7 +1909,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>43</v>
       </c>
@@ -2099,7 +1953,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>44</v>
       </c>
@@ -2143,7 +1997,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>45</v>
       </c>
@@ -2187,7 +2041,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>46</v>
       </c>
@@ -2231,7 +2085,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>47</v>
       </c>
@@ -2275,7 +2129,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>48</v>
       </c>
@@ -2319,7 +2173,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>49</v>
       </c>
@@ -2363,7 +2217,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>50</v>
       </c>
@@ -2407,7 +2261,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>51</v>
       </c>
@@ -2451,7 +2305,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>52</v>
       </c>
@@ -2495,7 +2349,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>53</v>
       </c>
@@ -2539,7 +2393,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>54</v>
       </c>
@@ -2583,7 +2437,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>55</v>
       </c>
@@ -2627,7 +2481,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>56</v>
       </c>
@@ -2671,7 +2525,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" ht="15.75" customHeight="1">
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>57</v>
       </c>
@@ -2715,7 +2569,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>58</v>
       </c>
@@ -2759,7 +2613,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" ht="15.75" customHeight="1">
+    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>59</v>
       </c>
@@ -2803,7 +2657,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" ht="15.75" customHeight="1">
+    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
         <v>60</v>
       </c>
@@ -2847,7 +2701,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" ht="15.75" customHeight="1">
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>61</v>
       </c>
@@ -2891,7 +2745,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" ht="15.75" customHeight="1">
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>62</v>
       </c>
@@ -2935,7 +2789,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" ht="15.75" customHeight="1">
+    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>63</v>
       </c>
@@ -2979,7 +2833,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" ht="15.75" customHeight="1">
+    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>64</v>
       </c>
@@ -3023,7 +2877,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" ht="15.75" customHeight="1">
+    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
         <v>65</v>
       </c>
@@ -3067,7 +2921,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" ht="15.75" customHeight="1">
+    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
         <v>66</v>
       </c>
@@ -3111,7 +2965,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" ht="15.75" customHeight="1">
+    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
         <v>67</v>
       </c>
@@ -3155,7 +3009,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" ht="15.75" customHeight="1">
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
         <v>68</v>
       </c>
@@ -3199,7 +3053,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" ht="15.75" customHeight="1">
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
         <v>69</v>
       </c>
@@ -3243,7 +3097,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" ht="15.75" customHeight="1">
+    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
         <v>70</v>
       </c>
@@ -3287,7 +3141,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" ht="15.75" customHeight="1">
+    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
         <v>71</v>
       </c>
@@ -3331,7 +3185,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" ht="15.75" customHeight="1">
+    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
         <v>72</v>
       </c>
@@ -3375,7 +3229,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" ht="15.75" customHeight="1">
+    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
         <v>73</v>
       </c>
@@ -3419,7 +3273,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" ht="15.75" customHeight="1">
+    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
         <v>74</v>
       </c>
@@ -3463,7 +3317,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" ht="15.75" customHeight="1">
+    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>75</v>
       </c>
@@ -3507,7 +3361,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" ht="15.75" customHeight="1">
+    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
         <v>76</v>
       </c>
@@ -3551,7 +3405,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" ht="15.75" customHeight="1">
+    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
         <v>77</v>
       </c>
@@ -3595,7 +3449,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" ht="15.75" customHeight="1">
+    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
         <v>78</v>
       </c>
@@ -3639,7 +3493,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" ht="15.75" customHeight="1">
+    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
         <v>79</v>
       </c>
@@ -3683,7 +3537,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65" ht="15.75" customHeight="1">
+    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
         <v>80</v>
       </c>
@@ -3727,7 +3581,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" ht="15.75" customHeight="1">
+    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
         <v>81</v>
       </c>
@@ -3771,7 +3625,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="67" ht="15.75" customHeight="1">
+    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
         <v>82</v>
       </c>
@@ -3815,7 +3669,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" ht="15.75" customHeight="1">
+    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
         <v>83</v>
       </c>
@@ -3859,7 +3713,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69" ht="15.75" customHeight="1">
+    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
         <v>84</v>
       </c>
@@ -3903,7 +3757,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" ht="15.75" customHeight="1">
+    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
         <v>85</v>
       </c>
@@ -3947,7 +3801,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="71" ht="15.75" customHeight="1">
+    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
         <v>86</v>
       </c>
@@ -3991,7 +3845,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="72" ht="15.75" customHeight="1">
+    <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
         <v>87</v>
       </c>
@@ -4035,7 +3889,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="73" ht="15.75" customHeight="1">
+    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
         <v>88</v>
       </c>
@@ -4079,7 +3933,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" ht="15.75" customHeight="1">
+    <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
         <v>89</v>
       </c>
@@ -4123,7 +3977,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" ht="15.75" customHeight="1">
+    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
         <v>90</v>
       </c>
@@ -4167,7 +4021,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" ht="15.75" customHeight="1">
+    <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
         <v>91</v>
       </c>
@@ -4211,7 +4065,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="77" ht="15.75" customHeight="1">
+    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
         <v>92</v>
       </c>
@@ -4255,7 +4109,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" ht="15.75" customHeight="1">
+    <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
         <v>93</v>
       </c>
@@ -4299,7 +4153,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="79" ht="15.75" customHeight="1">
+    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
         <v>94</v>
       </c>
@@ -4343,7 +4197,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="80" ht="15.75" customHeight="1">
+    <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
         <v>95</v>
       </c>
@@ -4387,7 +4241,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" ht="15.75" customHeight="1">
+    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
         <v>96</v>
       </c>
@@ -4431,7 +4285,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="82" ht="15.75" customHeight="1">
+    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
         <v>97</v>
       </c>
@@ -4475,7 +4329,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="83" ht="15.75" customHeight="1">
+    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
         <v>98</v>
       </c>
@@ -4519,7 +4373,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="84" ht="15.75" customHeight="1">
+    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
         <v>99</v>
       </c>
@@ -4563,7 +4417,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="85" ht="15.75" customHeight="1">
+    <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
         <v>100</v>
       </c>
@@ -4607,7 +4461,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="86" ht="15.75" customHeight="1">
+    <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
         <v>101</v>
       </c>
@@ -4651,7 +4505,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" ht="15.75" customHeight="1">
+    <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
         <v>102</v>
       </c>
@@ -4695,7 +4549,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="88" ht="15.75" customHeight="1">
+    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
         <v>103</v>
       </c>
@@ -4739,7 +4593,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="89" ht="15.75" customHeight="1">
+    <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
         <v>104</v>
       </c>
@@ -4783,7 +4637,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="90" ht="15.75" customHeight="1">
+    <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
         <v>105</v>
       </c>
@@ -4827,7 +4681,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="91" ht="15.75" customHeight="1">
+    <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
         <v>106</v>
       </c>
@@ -4871,7 +4725,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" ht="15.75" customHeight="1">
+    <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
         <v>107</v>
       </c>
@@ -4915,7 +4769,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="93" ht="15.75" customHeight="1">
+    <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
         <v>108</v>
       </c>
@@ -4959,7 +4813,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="94" ht="15.75" customHeight="1">
+    <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
         <v>109</v>
       </c>
@@ -5003,7 +4857,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="95" ht="15.75" customHeight="1">
+    <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
         <v>110</v>
       </c>
@@ -5047,7 +4901,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="96" ht="15.75" customHeight="1">
+    <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
         <v>111</v>
       </c>
@@ -5091,7 +4945,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="97" ht="15.75" customHeight="1">
+    <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
         <v>112</v>
       </c>
@@ -5135,7 +4989,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="98" ht="15.75" customHeight="1">
+    <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
         <v>113</v>
       </c>
@@ -5179,7 +5033,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="99" ht="15.75" customHeight="1">
+    <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
         <v>114</v>
       </c>
@@ -5223,7 +5077,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="100" ht="15.75" customHeight="1">
+    <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
         <v>115</v>
       </c>
@@ -5267,7 +5121,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="101" ht="15.75" customHeight="1">
+    <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
         <v>116</v>
       </c>
@@ -5311,7 +5165,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="102" ht="15.75" customHeight="1">
+    <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
         <v>117</v>
       </c>
@@ -5355,7 +5209,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="103" ht="15.75" customHeight="1">
+    <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
         <v>118</v>
       </c>
@@ -5399,7 +5253,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="104" ht="15.75" customHeight="1">
+    <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
         <v>119</v>
       </c>
@@ -5443,7 +5297,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="105" ht="15.75" customHeight="1">
+    <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
         <v>120</v>
       </c>
@@ -5487,7 +5341,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="106" ht="15.75" customHeight="1">
+    <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
         <v>121</v>
       </c>
@@ -5531,7 +5385,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="107" ht="15.75" customHeight="1">
+    <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
         <v>122</v>
       </c>
@@ -5575,7 +5429,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" ht="15.75" customHeight="1">
+    <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
         <v>123</v>
       </c>
@@ -5619,7 +5473,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" ht="15.75" customHeight="1">
+    <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
         <v>124</v>
       </c>
@@ -5663,7 +5517,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" ht="15.75" customHeight="1">
+    <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
         <v>125</v>
       </c>
@@ -5707,7 +5561,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="111" ht="15.75" customHeight="1">
+    <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
         <v>126</v>
       </c>
@@ -5751,7 +5605,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="112" ht="15.75" customHeight="1">
+    <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
         <v>127</v>
       </c>
@@ -5795,7 +5649,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="113" ht="15.75" customHeight="1">
+    <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
         <v>128</v>
       </c>
@@ -5839,7 +5693,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="114" ht="15.75" customHeight="1">
+    <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
         <v>129</v>
       </c>
@@ -5883,7 +5737,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="115" ht="15.75" customHeight="1">
+    <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
         <v>130</v>
       </c>
@@ -5927,7 +5781,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="116" ht="15.75" customHeight="1">
+    <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
         <v>131</v>
       </c>
@@ -5971,7 +5825,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="117" ht="15.75" customHeight="1">
+    <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
         <v>132</v>
       </c>
@@ -6015,7 +5869,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="118" ht="15.75" customHeight="1">
+    <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
         <v>133</v>
       </c>
@@ -6059,7 +5913,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="119" ht="15.75" customHeight="1">
+    <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
         <v>134</v>
       </c>
@@ -6103,7 +5957,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="120" ht="15.75" customHeight="1">
+    <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
         <v>135</v>
       </c>
@@ -6147,7 +6001,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="121" ht="15.75" customHeight="1">
+    <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
         <v>136</v>
       </c>
@@ -6191,7 +6045,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="122" ht="15.75" customHeight="1">
+    <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
         <v>137</v>
       </c>
@@ -6235,7 +6089,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="123" ht="15.75" customHeight="1">
+    <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
         <v>138</v>
       </c>
@@ -6279,7 +6133,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="124" ht="15.75" customHeight="1">
+    <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
         <v>139</v>
       </c>
@@ -6323,7 +6177,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="125" ht="15.75" customHeight="1">
+    <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
         <v>140</v>
       </c>
@@ -6367,7 +6221,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="126" ht="15.75" customHeight="1">
+    <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
         <v>141</v>
       </c>
@@ -6411,7 +6265,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="127" ht="15.75" customHeight="1">
+    <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
         <v>142</v>
       </c>
@@ -6455,7 +6309,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="128" ht="15.75" customHeight="1">
+    <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
         <v>143</v>
       </c>
@@ -6499,7 +6353,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="129" ht="15.75" customHeight="1">
+    <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
         <v>144</v>
       </c>
@@ -6543,7 +6397,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="130" ht="15.75" customHeight="1">
+    <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
         <v>145</v>
       </c>
@@ -6587,7 +6441,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="131" ht="15.75" customHeight="1">
+    <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
         <v>146</v>
       </c>
@@ -6631,7 +6485,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="132" ht="15.75" customHeight="1">
+    <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
         <v>147</v>
       </c>
@@ -6675,7 +6529,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="133" ht="15.75" customHeight="1">
+    <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
         <v>148</v>
       </c>
@@ -6719,7 +6573,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="134" ht="15.75" customHeight="1">
+    <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
         <v>149</v>
       </c>
@@ -6763,7 +6617,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="135" ht="15.75" customHeight="1">
+    <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
         <v>150</v>
       </c>
@@ -6807,7 +6661,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="136" ht="15.75" customHeight="1">
+    <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
         <v>151</v>
       </c>
@@ -6851,7 +6705,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="137" ht="15.75" customHeight="1">
+    <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
         <v>152</v>
       </c>
@@ -6895,7 +6749,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="138" ht="15.75" customHeight="1">
+    <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
         <v>153</v>
       </c>
@@ -6939,7 +6793,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="139" ht="15.75" customHeight="1">
+    <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
         <v>154</v>
       </c>
@@ -6983,7 +6837,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="140" ht="15.75" customHeight="1">
+    <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
         <v>155</v>
       </c>
@@ -7027,7 +6881,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="141" ht="15.75" customHeight="1">
+    <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
         <v>156</v>
       </c>
@@ -7071,7 +6925,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="142" ht="15.75" customHeight="1">
+    <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
         <v>157</v>
       </c>
@@ -7115,7 +6969,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="143" ht="15.75" customHeight="1">
+    <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
         <v>158</v>
       </c>
@@ -7159,7 +7013,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="144" ht="15.75" customHeight="1">
+    <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
         <v>159</v>
       </c>
@@ -7203,7 +7057,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="145" ht="15.75" customHeight="1">
+    <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
         <v>160</v>
       </c>
@@ -7247,7 +7101,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="146" ht="15.75" customHeight="1">
+    <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
         <v>161</v>
       </c>
@@ -7291,7 +7145,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="147" ht="15.75" customHeight="1">
+    <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
         <v>162</v>
       </c>
@@ -7335,7 +7189,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="148" ht="15.75" customHeight="1">
+    <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="s">
         <v>163</v>
       </c>
@@ -7379,7 +7233,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="149" ht="15.75" customHeight="1">
+    <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="s">
         <v>164</v>
       </c>
@@ -7423,7 +7277,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="150" ht="15.75" customHeight="1">
+    <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="1" t="s">
         <v>165</v>
       </c>
@@ -7467,7 +7321,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="151" ht="15.75" customHeight="1">
+    <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="1" t="s">
         <v>166</v>
       </c>
@@ -7511,7 +7365,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="152" ht="15.75" customHeight="1">
+    <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="s">
         <v>167</v>
       </c>
@@ -7555,7 +7409,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="153" ht="15.75" customHeight="1">
+    <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="1" t="s">
         <v>168</v>
       </c>
@@ -7599,7 +7453,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="154" ht="15.75" customHeight="1">
+    <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="s">
         <v>169</v>
       </c>
@@ -7643,7 +7497,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" ht="15.75" customHeight="1">
+    <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="s">
         <v>170</v>
       </c>
@@ -7687,7 +7541,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" ht="15.75" customHeight="1">
+    <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="s">
         <v>171</v>
       </c>
@@ -7731,7 +7585,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="157" ht="15.75" customHeight="1">
+    <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A157" s="1" t="s">
         <v>172</v>
       </c>
@@ -7775,7 +7629,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="158" ht="15.75" customHeight="1">
+    <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="1" t="s">
         <v>173</v>
       </c>
@@ -7819,7 +7673,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="159" ht="15.75" customHeight="1">
+    <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="s">
         <v>174</v>
       </c>
@@ -7863,7 +7717,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="160" ht="15.75" customHeight="1">
+    <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
         <v>175</v>
       </c>
@@ -7907,7 +7761,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="161" ht="15.75" customHeight="1">
+    <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="1" t="s">
         <v>176</v>
       </c>
@@ -7951,7 +7805,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="162" ht="15.75" customHeight="1">
+    <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="s">
         <v>177</v>
       </c>
@@ -7995,7 +7849,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" ht="15.75" customHeight="1">
+    <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="s">
         <v>178</v>
       </c>
@@ -8039,7 +7893,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="164" ht="15.75" customHeight="1">
+    <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="s">
         <v>179</v>
       </c>
@@ -8083,7 +7937,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" ht="15.75" customHeight="1">
+    <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="s">
         <v>180</v>
       </c>
@@ -8127,7 +7981,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" ht="15.75" customHeight="1">
+    <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="1" t="s">
         <v>181</v>
       </c>
@@ -8171,7 +8025,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" ht="15.75" customHeight="1">
+    <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="s">
         <v>182</v>
       </c>
@@ -8215,7 +8069,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" ht="15.75" customHeight="1">
+    <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="s">
         <v>183</v>
       </c>
@@ -8259,7 +8113,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" ht="15.75" customHeight="1">
+    <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="s">
         <v>184</v>
       </c>
@@ -8303,7 +8157,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" ht="15.75" customHeight="1">
+    <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="1" t="s">
         <v>185</v>
       </c>
@@ -8347,7 +8201,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" ht="15.75" customHeight="1">
+    <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="s">
         <v>186</v>
       </c>
@@ -8391,7 +8245,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="172" ht="15.75" customHeight="1">
+    <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="s">
         <v>187</v>
       </c>
@@ -8435,7 +8289,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="173" ht="15.75" customHeight="1">
+    <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A173" s="1" t="s">
         <v>188</v>
       </c>
@@ -8479,837 +8333,840 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" ht="15.75" customHeight="1"/>
-    <row r="175" ht="15.75" customHeight="1"/>
-    <row r="176" ht="15.75" customHeight="1"/>
-    <row r="177" ht="15.75" customHeight="1"/>
-    <row r="178" ht="15.75" customHeight="1"/>
-    <row r="179" ht="15.75" customHeight="1"/>
-    <row r="180" ht="15.75" customHeight="1"/>
-    <row r="181" ht="15.75" customHeight="1"/>
-    <row r="182" ht="15.75" customHeight="1"/>
-    <row r="183" ht="15.75" customHeight="1"/>
-    <row r="184" ht="15.75" customHeight="1"/>
-    <row r="185" ht="15.75" customHeight="1"/>
-    <row r="186" ht="15.75" customHeight="1"/>
-    <row r="187" ht="15.75" customHeight="1"/>
-    <row r="188" ht="15.75" customHeight="1"/>
-    <row r="189" ht="15.75" customHeight="1"/>
-    <row r="190" ht="15.75" customHeight="1"/>
-    <row r="191" ht="15.75" customHeight="1"/>
-    <row r="192" ht="15.75" customHeight="1"/>
-    <row r="193" ht="15.75" customHeight="1"/>
-    <row r="194" ht="15.75" customHeight="1"/>
-    <row r="195" ht="15.75" customHeight="1"/>
-    <row r="196" ht="15.75" customHeight="1"/>
-    <row r="197" ht="15.75" customHeight="1"/>
-    <row r="198" ht="15.75" customHeight="1"/>
-    <row r="199" ht="15.75" customHeight="1"/>
-    <row r="200" ht="15.75" customHeight="1"/>
-    <row r="201" ht="15.75" customHeight="1"/>
-    <row r="202" ht="15.75" customHeight="1"/>
-    <row r="203" ht="15.75" customHeight="1"/>
-    <row r="204" ht="15.75" customHeight="1"/>
-    <row r="205" ht="15.75" customHeight="1"/>
-    <row r="206" ht="15.75" customHeight="1"/>
-    <row r="207" ht="15.75" customHeight="1"/>
-    <row r="208" ht="15.75" customHeight="1"/>
-    <row r="209" ht="15.75" customHeight="1"/>
-    <row r="210" ht="15.75" customHeight="1"/>
-    <row r="211" ht="15.75" customHeight="1"/>
-    <row r="212" ht="15.75" customHeight="1"/>
-    <row r="213" ht="15.75" customHeight="1"/>
-    <row r="214" ht="15.75" customHeight="1"/>
-    <row r="215" ht="15.75" customHeight="1"/>
-    <row r="216" ht="15.75" customHeight="1"/>
-    <row r="217" ht="15.75" customHeight="1"/>
-    <row r="218" ht="15.75" customHeight="1"/>
-    <row r="219" ht="15.75" customHeight="1"/>
-    <row r="220" ht="15.75" customHeight="1"/>
-    <row r="221" ht="15.75" customHeight="1"/>
-    <row r="222" ht="15.75" customHeight="1"/>
-    <row r="223" ht="15.75" customHeight="1"/>
-    <row r="224" ht="15.75" customHeight="1"/>
-    <row r="225" ht="15.75" customHeight="1"/>
-    <row r="226" ht="15.75" customHeight="1"/>
-    <row r="227" ht="15.75" customHeight="1"/>
-    <row r="228" ht="15.75" customHeight="1"/>
-    <row r="229" ht="15.75" customHeight="1"/>
-    <row r="230" ht="15.75" customHeight="1"/>
-    <row r="231" ht="15.75" customHeight="1"/>
-    <row r="232" ht="15.75" customHeight="1"/>
-    <row r="233" ht="15.75" customHeight="1"/>
-    <row r="234" ht="15.75" customHeight="1"/>
-    <row r="235" ht="15.75" customHeight="1"/>
-    <row r="236" ht="15.75" customHeight="1"/>
-    <row r="237" ht="15.75" customHeight="1"/>
-    <row r="238" ht="15.75" customHeight="1"/>
-    <row r="239" ht="15.75" customHeight="1"/>
-    <row r="240" ht="15.75" customHeight="1"/>
-    <row r="241" ht="15.75" customHeight="1"/>
-    <row r="242" ht="15.75" customHeight="1"/>
-    <row r="243" ht="15.75" customHeight="1"/>
-    <row r="244" ht="15.75" customHeight="1"/>
-    <row r="245" ht="15.75" customHeight="1"/>
-    <row r="246" ht="15.75" customHeight="1"/>
-    <row r="247" ht="15.75" customHeight="1"/>
-    <row r="248" ht="15.75" customHeight="1"/>
-    <row r="249" ht="15.75" customHeight="1"/>
-    <row r="250" ht="15.75" customHeight="1"/>
-    <row r="251" ht="15.75" customHeight="1"/>
-    <row r="252" ht="15.75" customHeight="1"/>
-    <row r="253" ht="15.75" customHeight="1"/>
-    <row r="254" ht="15.75" customHeight="1"/>
-    <row r="255" ht="15.75" customHeight="1"/>
-    <row r="256" ht="15.75" customHeight="1"/>
-    <row r="257" ht="15.75" customHeight="1"/>
-    <row r="258" ht="15.75" customHeight="1"/>
-    <row r="259" ht="15.75" customHeight="1"/>
-    <row r="260" ht="15.75" customHeight="1"/>
-    <row r="261" ht="15.75" customHeight="1"/>
-    <row r="262" ht="15.75" customHeight="1"/>
-    <row r="263" ht="15.75" customHeight="1"/>
-    <row r="264" ht="15.75" customHeight="1"/>
-    <row r="265" ht="15.75" customHeight="1"/>
-    <row r="266" ht="15.75" customHeight="1"/>
-    <row r="267" ht="15.75" customHeight="1"/>
-    <row r="268" ht="15.75" customHeight="1"/>
-    <row r="269" ht="15.75" customHeight="1"/>
-    <row r="270" ht="15.75" customHeight="1"/>
-    <row r="271" ht="15.75" customHeight="1"/>
-    <row r="272" ht="15.75" customHeight="1"/>
-    <row r="273" ht="15.75" customHeight="1"/>
-    <row r="274" ht="15.75" customHeight="1"/>
-    <row r="275" ht="15.75" customHeight="1"/>
-    <row r="276" ht="15.75" customHeight="1"/>
-    <row r="277" ht="15.75" customHeight="1"/>
-    <row r="278" ht="15.75" customHeight="1"/>
-    <row r="279" ht="15.75" customHeight="1"/>
-    <row r="280" ht="15.75" customHeight="1"/>
-    <row r="281" ht="15.75" customHeight="1"/>
-    <row r="282" ht="15.75" customHeight="1"/>
-    <row r="283" ht="15.75" customHeight="1"/>
-    <row r="284" ht="15.75" customHeight="1"/>
-    <row r="285" ht="15.75" customHeight="1"/>
-    <row r="286" ht="15.75" customHeight="1"/>
-    <row r="287" ht="15.75" customHeight="1"/>
-    <row r="288" ht="15.75" customHeight="1"/>
-    <row r="289" ht="15.75" customHeight="1"/>
-    <row r="290" ht="15.75" customHeight="1"/>
-    <row r="291" ht="15.75" customHeight="1"/>
-    <row r="292" ht="15.75" customHeight="1"/>
-    <row r="293" ht="15.75" customHeight="1"/>
-    <row r="294" ht="15.75" customHeight="1"/>
-    <row r="295" ht="15.75" customHeight="1"/>
-    <row r="296" ht="15.75" customHeight="1"/>
-    <row r="297" ht="15.75" customHeight="1"/>
-    <row r="298" ht="15.75" customHeight="1"/>
-    <row r="299" ht="15.75" customHeight="1"/>
-    <row r="300" ht="15.75" customHeight="1"/>
-    <row r="301" ht="15.75" customHeight="1"/>
-    <row r="302" ht="15.75" customHeight="1"/>
-    <row r="303" ht="15.75" customHeight="1"/>
-    <row r="304" ht="15.75" customHeight="1"/>
-    <row r="305" ht="15.75" customHeight="1"/>
-    <row r="306" ht="15.75" customHeight="1"/>
-    <row r="307" ht="15.75" customHeight="1"/>
-    <row r="308" ht="15.75" customHeight="1"/>
-    <row r="309" ht="15.75" customHeight="1"/>
-    <row r="310" ht="15.75" customHeight="1"/>
-    <row r="311" ht="15.75" customHeight="1"/>
-    <row r="312" ht="15.75" customHeight="1"/>
-    <row r="313" ht="15.75" customHeight="1"/>
-    <row r="314" ht="15.75" customHeight="1"/>
-    <row r="315" ht="15.75" customHeight="1"/>
-    <row r="316" ht="15.75" customHeight="1"/>
-    <row r="317" ht="15.75" customHeight="1"/>
-    <row r="318" ht="15.75" customHeight="1"/>
-    <row r="319" ht="15.75" customHeight="1"/>
-    <row r="320" ht="15.75" customHeight="1"/>
-    <row r="321" ht="15.75" customHeight="1"/>
-    <row r="322" ht="15.75" customHeight="1"/>
-    <row r="323" ht="15.75" customHeight="1"/>
-    <row r="324" ht="15.75" customHeight="1"/>
-    <row r="325" ht="15.75" customHeight="1"/>
-    <row r="326" ht="15.75" customHeight="1"/>
-    <row r="327" ht="15.75" customHeight="1"/>
-    <row r="328" ht="15.75" customHeight="1"/>
-    <row r="329" ht="15.75" customHeight="1"/>
-    <row r="330" ht="15.75" customHeight="1"/>
-    <row r="331" ht="15.75" customHeight="1"/>
-    <row r="332" ht="15.75" customHeight="1"/>
-    <row r="333" ht="15.75" customHeight="1"/>
-    <row r="334" ht="15.75" customHeight="1"/>
-    <row r="335" ht="15.75" customHeight="1"/>
-    <row r="336" ht="15.75" customHeight="1"/>
-    <row r="337" ht="15.75" customHeight="1"/>
-    <row r="338" ht="15.75" customHeight="1"/>
-    <row r="339" ht="15.75" customHeight="1"/>
-    <row r="340" ht="15.75" customHeight="1"/>
-    <row r="341" ht="15.75" customHeight="1"/>
-    <row r="342" ht="15.75" customHeight="1"/>
-    <row r="343" ht="15.75" customHeight="1"/>
-    <row r="344" ht="15.75" customHeight="1"/>
-    <row r="345" ht="15.75" customHeight="1"/>
-    <row r="346" ht="15.75" customHeight="1"/>
-    <row r="347" ht="15.75" customHeight="1"/>
-    <row r="348" ht="15.75" customHeight="1"/>
-    <row r="349" ht="15.75" customHeight="1"/>
-    <row r="350" ht="15.75" customHeight="1"/>
-    <row r="351" ht="15.75" customHeight="1"/>
-    <row r="352" ht="15.75" customHeight="1"/>
-    <row r="353" ht="15.75" customHeight="1"/>
-    <row r="354" ht="15.75" customHeight="1"/>
-    <row r="355" ht="15.75" customHeight="1"/>
-    <row r="356" ht="15.75" customHeight="1"/>
-    <row r="357" ht="15.75" customHeight="1"/>
-    <row r="358" ht="15.75" customHeight="1"/>
-    <row r="359" ht="15.75" customHeight="1"/>
-    <row r="360" ht="15.75" customHeight="1"/>
-    <row r="361" ht="15.75" customHeight="1"/>
-    <row r="362" ht="15.75" customHeight="1"/>
-    <row r="363" ht="15.75" customHeight="1"/>
-    <row r="364" ht="15.75" customHeight="1"/>
-    <row r="365" ht="15.75" customHeight="1"/>
-    <row r="366" ht="15.75" customHeight="1"/>
-    <row r="367" ht="15.75" customHeight="1"/>
-    <row r="368" ht="15.75" customHeight="1"/>
-    <row r="369" ht="15.75" customHeight="1"/>
-    <row r="370" ht="15.75" customHeight="1"/>
-    <row r="371" ht="15.75" customHeight="1"/>
-    <row r="372" ht="15.75" customHeight="1"/>
-    <row r="373" ht="15.75" customHeight="1"/>
-    <row r="374" ht="15.75" customHeight="1"/>
-    <row r="375" ht="15.75" customHeight="1"/>
-    <row r="376" ht="15.75" customHeight="1"/>
-    <row r="377" ht="15.75" customHeight="1"/>
-    <row r="378" ht="15.75" customHeight="1"/>
-    <row r="379" ht="15.75" customHeight="1"/>
-    <row r="380" ht="15.75" customHeight="1"/>
-    <row r="381" ht="15.75" customHeight="1"/>
-    <row r="382" ht="15.75" customHeight="1"/>
-    <row r="383" ht="15.75" customHeight="1"/>
-    <row r="384" ht="15.75" customHeight="1"/>
-    <row r="385" ht="15.75" customHeight="1"/>
-    <row r="386" ht="15.75" customHeight="1"/>
-    <row r="387" ht="15.75" customHeight="1"/>
-    <row r="388" ht="15.75" customHeight="1"/>
-    <row r="389" ht="15.75" customHeight="1"/>
-    <row r="390" ht="15.75" customHeight="1"/>
-    <row r="391" ht="15.75" customHeight="1"/>
-    <row r="392" ht="15.75" customHeight="1"/>
-    <row r="393" ht="15.75" customHeight="1"/>
-    <row r="394" ht="15.75" customHeight="1"/>
-    <row r="395" ht="15.75" customHeight="1"/>
-    <row r="396" ht="15.75" customHeight="1"/>
-    <row r="397" ht="15.75" customHeight="1"/>
-    <row r="398" ht="15.75" customHeight="1"/>
-    <row r="399" ht="15.75" customHeight="1"/>
-    <row r="400" ht="15.75" customHeight="1"/>
-    <row r="401" ht="15.75" customHeight="1"/>
-    <row r="402" ht="15.75" customHeight="1"/>
-    <row r="403" ht="15.75" customHeight="1"/>
-    <row r="404" ht="15.75" customHeight="1"/>
-    <row r="405" ht="15.75" customHeight="1"/>
-    <row r="406" ht="15.75" customHeight="1"/>
-    <row r="407" ht="15.75" customHeight="1"/>
-    <row r="408" ht="15.75" customHeight="1"/>
-    <row r="409" ht="15.75" customHeight="1"/>
-    <row r="410" ht="15.75" customHeight="1"/>
-    <row r="411" ht="15.75" customHeight="1"/>
-    <row r="412" ht="15.75" customHeight="1"/>
-    <row r="413" ht="15.75" customHeight="1"/>
-    <row r="414" ht="15.75" customHeight="1"/>
-    <row r="415" ht="15.75" customHeight="1"/>
-    <row r="416" ht="15.75" customHeight="1"/>
-    <row r="417" ht="15.75" customHeight="1"/>
-    <row r="418" ht="15.75" customHeight="1"/>
-    <row r="419" ht="15.75" customHeight="1"/>
-    <row r="420" ht="15.75" customHeight="1"/>
-    <row r="421" ht="15.75" customHeight="1"/>
-    <row r="422" ht="15.75" customHeight="1"/>
-    <row r="423" ht="15.75" customHeight="1"/>
-    <row r="424" ht="15.75" customHeight="1"/>
-    <row r="425" ht="15.75" customHeight="1"/>
-    <row r="426" ht="15.75" customHeight="1"/>
-    <row r="427" ht="15.75" customHeight="1"/>
-    <row r="428" ht="15.75" customHeight="1"/>
-    <row r="429" ht="15.75" customHeight="1"/>
-    <row r="430" ht="15.75" customHeight="1"/>
-    <row r="431" ht="15.75" customHeight="1"/>
-    <row r="432" ht="15.75" customHeight="1"/>
-    <row r="433" ht="15.75" customHeight="1"/>
-    <row r="434" ht="15.75" customHeight="1"/>
-    <row r="435" ht="15.75" customHeight="1"/>
-    <row r="436" ht="15.75" customHeight="1"/>
-    <row r="437" ht="15.75" customHeight="1"/>
-    <row r="438" ht="15.75" customHeight="1"/>
-    <row r="439" ht="15.75" customHeight="1"/>
-    <row r="440" ht="15.75" customHeight="1"/>
-    <row r="441" ht="15.75" customHeight="1"/>
-    <row r="442" ht="15.75" customHeight="1"/>
-    <row r="443" ht="15.75" customHeight="1"/>
-    <row r="444" ht="15.75" customHeight="1"/>
-    <row r="445" ht="15.75" customHeight="1"/>
-    <row r="446" ht="15.75" customHeight="1"/>
-    <row r="447" ht="15.75" customHeight="1"/>
-    <row r="448" ht="15.75" customHeight="1"/>
-    <row r="449" ht="15.75" customHeight="1"/>
-    <row r="450" ht="15.75" customHeight="1"/>
-    <row r="451" ht="15.75" customHeight="1"/>
-    <row r="452" ht="15.75" customHeight="1"/>
-    <row r="453" ht="15.75" customHeight="1"/>
-    <row r="454" ht="15.75" customHeight="1"/>
-    <row r="455" ht="15.75" customHeight="1"/>
-    <row r="456" ht="15.75" customHeight="1"/>
-    <row r="457" ht="15.75" customHeight="1"/>
-    <row r="458" ht="15.75" customHeight="1"/>
-    <row r="459" ht="15.75" customHeight="1"/>
-    <row r="460" ht="15.75" customHeight="1"/>
-    <row r="461" ht="15.75" customHeight="1"/>
-    <row r="462" ht="15.75" customHeight="1"/>
-    <row r="463" ht="15.75" customHeight="1"/>
-    <row r="464" ht="15.75" customHeight="1"/>
-    <row r="465" ht="15.75" customHeight="1"/>
-    <row r="466" ht="15.75" customHeight="1"/>
-    <row r="467" ht="15.75" customHeight="1"/>
-    <row r="468" ht="15.75" customHeight="1"/>
-    <row r="469" ht="15.75" customHeight="1"/>
-    <row r="470" ht="15.75" customHeight="1"/>
-    <row r="471" ht="15.75" customHeight="1"/>
-    <row r="472" ht="15.75" customHeight="1"/>
-    <row r="473" ht="15.75" customHeight="1"/>
-    <row r="474" ht="15.75" customHeight="1"/>
-    <row r="475" ht="15.75" customHeight="1"/>
-    <row r="476" ht="15.75" customHeight="1"/>
-    <row r="477" ht="15.75" customHeight="1"/>
-    <row r="478" ht="15.75" customHeight="1"/>
-    <row r="479" ht="15.75" customHeight="1"/>
-    <row r="480" ht="15.75" customHeight="1"/>
-    <row r="481" ht="15.75" customHeight="1"/>
-    <row r="482" ht="15.75" customHeight="1"/>
-    <row r="483" ht="15.75" customHeight="1"/>
-    <row r="484" ht="15.75" customHeight="1"/>
-    <row r="485" ht="15.75" customHeight="1"/>
-    <row r="486" ht="15.75" customHeight="1"/>
-    <row r="487" ht="15.75" customHeight="1"/>
-    <row r="488" ht="15.75" customHeight="1"/>
-    <row r="489" ht="15.75" customHeight="1"/>
-    <row r="490" ht="15.75" customHeight="1"/>
-    <row r="491" ht="15.75" customHeight="1"/>
-    <row r="492" ht="15.75" customHeight="1"/>
-    <row r="493" ht="15.75" customHeight="1"/>
-    <row r="494" ht="15.75" customHeight="1"/>
-    <row r="495" ht="15.75" customHeight="1"/>
-    <row r="496" ht="15.75" customHeight="1"/>
-    <row r="497" ht="15.75" customHeight="1"/>
-    <row r="498" ht="15.75" customHeight="1"/>
-    <row r="499" ht="15.75" customHeight="1"/>
-    <row r="500" ht="15.75" customHeight="1"/>
-    <row r="501" ht="15.75" customHeight="1"/>
-    <row r="502" ht="15.75" customHeight="1"/>
-    <row r="503" ht="15.75" customHeight="1"/>
-    <row r="504" ht="15.75" customHeight="1"/>
-    <row r="505" ht="15.75" customHeight="1"/>
-    <row r="506" ht="15.75" customHeight="1"/>
-    <row r="507" ht="15.75" customHeight="1"/>
-    <row r="508" ht="15.75" customHeight="1"/>
-    <row r="509" ht="15.75" customHeight="1"/>
-    <row r="510" ht="15.75" customHeight="1"/>
-    <row r="511" ht="15.75" customHeight="1"/>
-    <row r="512" ht="15.75" customHeight="1"/>
-    <row r="513" ht="15.75" customHeight="1"/>
-    <row r="514" ht="15.75" customHeight="1"/>
-    <row r="515" ht="15.75" customHeight="1"/>
-    <row r="516" ht="15.75" customHeight="1"/>
-    <row r="517" ht="15.75" customHeight="1"/>
-    <row r="518" ht="15.75" customHeight="1"/>
-    <row r="519" ht="15.75" customHeight="1"/>
-    <row r="520" ht="15.75" customHeight="1"/>
-    <row r="521" ht="15.75" customHeight="1"/>
-    <row r="522" ht="15.75" customHeight="1"/>
-    <row r="523" ht="15.75" customHeight="1"/>
-    <row r="524" ht="15.75" customHeight="1"/>
-    <row r="525" ht="15.75" customHeight="1"/>
-    <row r="526" ht="15.75" customHeight="1"/>
-    <row r="527" ht="15.75" customHeight="1"/>
-    <row r="528" ht="15.75" customHeight="1"/>
-    <row r="529" ht="15.75" customHeight="1"/>
-    <row r="530" ht="15.75" customHeight="1"/>
-    <row r="531" ht="15.75" customHeight="1"/>
-    <row r="532" ht="15.75" customHeight="1"/>
-    <row r="533" ht="15.75" customHeight="1"/>
-    <row r="534" ht="15.75" customHeight="1"/>
-    <row r="535" ht="15.75" customHeight="1"/>
-    <row r="536" ht="15.75" customHeight="1"/>
-    <row r="537" ht="15.75" customHeight="1"/>
-    <row r="538" ht="15.75" customHeight="1"/>
-    <row r="539" ht="15.75" customHeight="1"/>
-    <row r="540" ht="15.75" customHeight="1"/>
-    <row r="541" ht="15.75" customHeight="1"/>
-    <row r="542" ht="15.75" customHeight="1"/>
-    <row r="543" ht="15.75" customHeight="1"/>
-    <row r="544" ht="15.75" customHeight="1"/>
-    <row r="545" ht="15.75" customHeight="1"/>
-    <row r="546" ht="15.75" customHeight="1"/>
-    <row r="547" ht="15.75" customHeight="1"/>
-    <row r="548" ht="15.75" customHeight="1"/>
-    <row r="549" ht="15.75" customHeight="1"/>
-    <row r="550" ht="15.75" customHeight="1"/>
-    <row r="551" ht="15.75" customHeight="1"/>
-    <row r="552" ht="15.75" customHeight="1"/>
-    <row r="553" ht="15.75" customHeight="1"/>
-    <row r="554" ht="15.75" customHeight="1"/>
-    <row r="555" ht="15.75" customHeight="1"/>
-    <row r="556" ht="15.75" customHeight="1"/>
-    <row r="557" ht="15.75" customHeight="1"/>
-    <row r="558" ht="15.75" customHeight="1"/>
-    <row r="559" ht="15.75" customHeight="1"/>
-    <row r="560" ht="15.75" customHeight="1"/>
-    <row r="561" ht="15.75" customHeight="1"/>
-    <row r="562" ht="15.75" customHeight="1"/>
-    <row r="563" ht="15.75" customHeight="1"/>
-    <row r="564" ht="15.75" customHeight="1"/>
-    <row r="565" ht="15.75" customHeight="1"/>
-    <row r="566" ht="15.75" customHeight="1"/>
-    <row r="567" ht="15.75" customHeight="1"/>
-    <row r="568" ht="15.75" customHeight="1"/>
-    <row r="569" ht="15.75" customHeight="1"/>
-    <row r="570" ht="15.75" customHeight="1"/>
-    <row r="571" ht="15.75" customHeight="1"/>
-    <row r="572" ht="15.75" customHeight="1"/>
-    <row r="573" ht="15.75" customHeight="1"/>
-    <row r="574" ht="15.75" customHeight="1"/>
-    <row r="575" ht="15.75" customHeight="1"/>
-    <row r="576" ht="15.75" customHeight="1"/>
-    <row r="577" ht="15.75" customHeight="1"/>
-    <row r="578" ht="15.75" customHeight="1"/>
-    <row r="579" ht="15.75" customHeight="1"/>
-    <row r="580" ht="15.75" customHeight="1"/>
-    <row r="581" ht="15.75" customHeight="1"/>
-    <row r="582" ht="15.75" customHeight="1"/>
-    <row r="583" ht="15.75" customHeight="1"/>
-    <row r="584" ht="15.75" customHeight="1"/>
-    <row r="585" ht="15.75" customHeight="1"/>
-    <row r="586" ht="15.75" customHeight="1"/>
-    <row r="587" ht="15.75" customHeight="1"/>
-    <row r="588" ht="15.75" customHeight="1"/>
-    <row r="589" ht="15.75" customHeight="1"/>
-    <row r="590" ht="15.75" customHeight="1"/>
-    <row r="591" ht="15.75" customHeight="1"/>
-    <row r="592" ht="15.75" customHeight="1"/>
-    <row r="593" ht="15.75" customHeight="1"/>
-    <row r="594" ht="15.75" customHeight="1"/>
-    <row r="595" ht="15.75" customHeight="1"/>
-    <row r="596" ht="15.75" customHeight="1"/>
-    <row r="597" ht="15.75" customHeight="1"/>
-    <row r="598" ht="15.75" customHeight="1"/>
-    <row r="599" ht="15.75" customHeight="1"/>
-    <row r="600" ht="15.75" customHeight="1"/>
-    <row r="601" ht="15.75" customHeight="1"/>
-    <row r="602" ht="15.75" customHeight="1"/>
-    <row r="603" ht="15.75" customHeight="1"/>
-    <row r="604" ht="15.75" customHeight="1"/>
-    <row r="605" ht="15.75" customHeight="1"/>
-    <row r="606" ht="15.75" customHeight="1"/>
-    <row r="607" ht="15.75" customHeight="1"/>
-    <row r="608" ht="15.75" customHeight="1"/>
-    <row r="609" ht="15.75" customHeight="1"/>
-    <row r="610" ht="15.75" customHeight="1"/>
-    <row r="611" ht="15.75" customHeight="1"/>
-    <row r="612" ht="15.75" customHeight="1"/>
-    <row r="613" ht="15.75" customHeight="1"/>
-    <row r="614" ht="15.75" customHeight="1"/>
-    <row r="615" ht="15.75" customHeight="1"/>
-    <row r="616" ht="15.75" customHeight="1"/>
-    <row r="617" ht="15.75" customHeight="1"/>
-    <row r="618" ht="15.75" customHeight="1"/>
-    <row r="619" ht="15.75" customHeight="1"/>
-    <row r="620" ht="15.75" customHeight="1"/>
-    <row r="621" ht="15.75" customHeight="1"/>
-    <row r="622" ht="15.75" customHeight="1"/>
-    <row r="623" ht="15.75" customHeight="1"/>
-    <row r="624" ht="15.75" customHeight="1"/>
-    <row r="625" ht="15.75" customHeight="1"/>
-    <row r="626" ht="15.75" customHeight="1"/>
-    <row r="627" ht="15.75" customHeight="1"/>
-    <row r="628" ht="15.75" customHeight="1"/>
-    <row r="629" ht="15.75" customHeight="1"/>
-    <row r="630" ht="15.75" customHeight="1"/>
-    <row r="631" ht="15.75" customHeight="1"/>
-    <row r="632" ht="15.75" customHeight="1"/>
-    <row r="633" ht="15.75" customHeight="1"/>
-    <row r="634" ht="15.75" customHeight="1"/>
-    <row r="635" ht="15.75" customHeight="1"/>
-    <row r="636" ht="15.75" customHeight="1"/>
-    <row r="637" ht="15.75" customHeight="1"/>
-    <row r="638" ht="15.75" customHeight="1"/>
-    <row r="639" ht="15.75" customHeight="1"/>
-    <row r="640" ht="15.75" customHeight="1"/>
-    <row r="641" ht="15.75" customHeight="1"/>
-    <row r="642" ht="15.75" customHeight="1"/>
-    <row r="643" ht="15.75" customHeight="1"/>
-    <row r="644" ht="15.75" customHeight="1"/>
-    <row r="645" ht="15.75" customHeight="1"/>
-    <row r="646" ht="15.75" customHeight="1"/>
-    <row r="647" ht="15.75" customHeight="1"/>
-    <row r="648" ht="15.75" customHeight="1"/>
-    <row r="649" ht="15.75" customHeight="1"/>
-    <row r="650" ht="15.75" customHeight="1"/>
-    <row r="651" ht="15.75" customHeight="1"/>
-    <row r="652" ht="15.75" customHeight="1"/>
-    <row r="653" ht="15.75" customHeight="1"/>
-    <row r="654" ht="15.75" customHeight="1"/>
-    <row r="655" ht="15.75" customHeight="1"/>
-    <row r="656" ht="15.75" customHeight="1"/>
-    <row r="657" ht="15.75" customHeight="1"/>
-    <row r="658" ht="15.75" customHeight="1"/>
-    <row r="659" ht="15.75" customHeight="1"/>
-    <row r="660" ht="15.75" customHeight="1"/>
-    <row r="661" ht="15.75" customHeight="1"/>
-    <row r="662" ht="15.75" customHeight="1"/>
-    <row r="663" ht="15.75" customHeight="1"/>
-    <row r="664" ht="15.75" customHeight="1"/>
-    <row r="665" ht="15.75" customHeight="1"/>
-    <row r="666" ht="15.75" customHeight="1"/>
-    <row r="667" ht="15.75" customHeight="1"/>
-    <row r="668" ht="15.75" customHeight="1"/>
-    <row r="669" ht="15.75" customHeight="1"/>
-    <row r="670" ht="15.75" customHeight="1"/>
-    <row r="671" ht="15.75" customHeight="1"/>
-    <row r="672" ht="15.75" customHeight="1"/>
-    <row r="673" ht="15.75" customHeight="1"/>
-    <row r="674" ht="15.75" customHeight="1"/>
-    <row r="675" ht="15.75" customHeight="1"/>
-    <row r="676" ht="15.75" customHeight="1"/>
-    <row r="677" ht="15.75" customHeight="1"/>
-    <row r="678" ht="15.75" customHeight="1"/>
-    <row r="679" ht="15.75" customHeight="1"/>
-    <row r="680" ht="15.75" customHeight="1"/>
-    <row r="681" ht="15.75" customHeight="1"/>
-    <row r="682" ht="15.75" customHeight="1"/>
-    <row r="683" ht="15.75" customHeight="1"/>
-    <row r="684" ht="15.75" customHeight="1"/>
-    <row r="685" ht="15.75" customHeight="1"/>
-    <row r="686" ht="15.75" customHeight="1"/>
-    <row r="687" ht="15.75" customHeight="1"/>
-    <row r="688" ht="15.75" customHeight="1"/>
-    <row r="689" ht="15.75" customHeight="1"/>
-    <row r="690" ht="15.75" customHeight="1"/>
-    <row r="691" ht="15.75" customHeight="1"/>
-    <row r="692" ht="15.75" customHeight="1"/>
-    <row r="693" ht="15.75" customHeight="1"/>
-    <row r="694" ht="15.75" customHeight="1"/>
-    <row r="695" ht="15.75" customHeight="1"/>
-    <row r="696" ht="15.75" customHeight="1"/>
-    <row r="697" ht="15.75" customHeight="1"/>
-    <row r="698" ht="15.75" customHeight="1"/>
-    <row r="699" ht="15.75" customHeight="1"/>
-    <row r="700" ht="15.75" customHeight="1"/>
-    <row r="701" ht="15.75" customHeight="1"/>
-    <row r="702" ht="15.75" customHeight="1"/>
-    <row r="703" ht="15.75" customHeight="1"/>
-    <row r="704" ht="15.75" customHeight="1"/>
-    <row r="705" ht="15.75" customHeight="1"/>
-    <row r="706" ht="15.75" customHeight="1"/>
-    <row r="707" ht="15.75" customHeight="1"/>
-    <row r="708" ht="15.75" customHeight="1"/>
-    <row r="709" ht="15.75" customHeight="1"/>
-    <row r="710" ht="15.75" customHeight="1"/>
-    <row r="711" ht="15.75" customHeight="1"/>
-    <row r="712" ht="15.75" customHeight="1"/>
-    <row r="713" ht="15.75" customHeight="1"/>
-    <row r="714" ht="15.75" customHeight="1"/>
-    <row r="715" ht="15.75" customHeight="1"/>
-    <row r="716" ht="15.75" customHeight="1"/>
-    <row r="717" ht="15.75" customHeight="1"/>
-    <row r="718" ht="15.75" customHeight="1"/>
-    <row r="719" ht="15.75" customHeight="1"/>
-    <row r="720" ht="15.75" customHeight="1"/>
-    <row r="721" ht="15.75" customHeight="1"/>
-    <row r="722" ht="15.75" customHeight="1"/>
-    <row r="723" ht="15.75" customHeight="1"/>
-    <row r="724" ht="15.75" customHeight="1"/>
-    <row r="725" ht="15.75" customHeight="1"/>
-    <row r="726" ht="15.75" customHeight="1"/>
-    <row r="727" ht="15.75" customHeight="1"/>
-    <row r="728" ht="15.75" customHeight="1"/>
-    <row r="729" ht="15.75" customHeight="1"/>
-    <row r="730" ht="15.75" customHeight="1"/>
-    <row r="731" ht="15.75" customHeight="1"/>
-    <row r="732" ht="15.75" customHeight="1"/>
-    <row r="733" ht="15.75" customHeight="1"/>
-    <row r="734" ht="15.75" customHeight="1"/>
-    <row r="735" ht="15.75" customHeight="1"/>
-    <row r="736" ht="15.75" customHeight="1"/>
-    <row r="737" ht="15.75" customHeight="1"/>
-    <row r="738" ht="15.75" customHeight="1"/>
-    <row r="739" ht="15.75" customHeight="1"/>
-    <row r="740" ht="15.75" customHeight="1"/>
-    <row r="741" ht="15.75" customHeight="1"/>
-    <row r="742" ht="15.75" customHeight="1"/>
-    <row r="743" ht="15.75" customHeight="1"/>
-    <row r="744" ht="15.75" customHeight="1"/>
-    <row r="745" ht="15.75" customHeight="1"/>
-    <row r="746" ht="15.75" customHeight="1"/>
-    <row r="747" ht="15.75" customHeight="1"/>
-    <row r="748" ht="15.75" customHeight="1"/>
-    <row r="749" ht="15.75" customHeight="1"/>
-    <row r="750" ht="15.75" customHeight="1"/>
-    <row r="751" ht="15.75" customHeight="1"/>
-    <row r="752" ht="15.75" customHeight="1"/>
-    <row r="753" ht="15.75" customHeight="1"/>
-    <row r="754" ht="15.75" customHeight="1"/>
-    <row r="755" ht="15.75" customHeight="1"/>
-    <row r="756" ht="15.75" customHeight="1"/>
-    <row r="757" ht="15.75" customHeight="1"/>
-    <row r="758" ht="15.75" customHeight="1"/>
-    <row r="759" ht="15.75" customHeight="1"/>
-    <row r="760" ht="15.75" customHeight="1"/>
-    <row r="761" ht="15.75" customHeight="1"/>
-    <row r="762" ht="15.75" customHeight="1"/>
-    <row r="763" ht="15.75" customHeight="1"/>
-    <row r="764" ht="15.75" customHeight="1"/>
-    <row r="765" ht="15.75" customHeight="1"/>
-    <row r="766" ht="15.75" customHeight="1"/>
-    <row r="767" ht="15.75" customHeight="1"/>
-    <row r="768" ht="15.75" customHeight="1"/>
-    <row r="769" ht="15.75" customHeight="1"/>
-    <row r="770" ht="15.75" customHeight="1"/>
-    <row r="771" ht="15.75" customHeight="1"/>
-    <row r="772" ht="15.75" customHeight="1"/>
-    <row r="773" ht="15.75" customHeight="1"/>
-    <row r="774" ht="15.75" customHeight="1"/>
-    <row r="775" ht="15.75" customHeight="1"/>
-    <row r="776" ht="15.75" customHeight="1"/>
-    <row r="777" ht="15.75" customHeight="1"/>
-    <row r="778" ht="15.75" customHeight="1"/>
-    <row r="779" ht="15.75" customHeight="1"/>
-    <row r="780" ht="15.75" customHeight="1"/>
-    <row r="781" ht="15.75" customHeight="1"/>
-    <row r="782" ht="15.75" customHeight="1"/>
-    <row r="783" ht="15.75" customHeight="1"/>
-    <row r="784" ht="15.75" customHeight="1"/>
-    <row r="785" ht="15.75" customHeight="1"/>
-    <row r="786" ht="15.75" customHeight="1"/>
-    <row r="787" ht="15.75" customHeight="1"/>
-    <row r="788" ht="15.75" customHeight="1"/>
-    <row r="789" ht="15.75" customHeight="1"/>
-    <row r="790" ht="15.75" customHeight="1"/>
-    <row r="791" ht="15.75" customHeight="1"/>
-    <row r="792" ht="15.75" customHeight="1"/>
-    <row r="793" ht="15.75" customHeight="1"/>
-    <row r="794" ht="15.75" customHeight="1"/>
-    <row r="795" ht="15.75" customHeight="1"/>
-    <row r="796" ht="15.75" customHeight="1"/>
-    <row r="797" ht="15.75" customHeight="1"/>
-    <row r="798" ht="15.75" customHeight="1"/>
-    <row r="799" ht="15.75" customHeight="1"/>
-    <row r="800" ht="15.75" customHeight="1"/>
-    <row r="801" ht="15.75" customHeight="1"/>
-    <row r="802" ht="15.75" customHeight="1"/>
-    <row r="803" ht="15.75" customHeight="1"/>
-    <row r="804" ht="15.75" customHeight="1"/>
-    <row r="805" ht="15.75" customHeight="1"/>
-    <row r="806" ht="15.75" customHeight="1"/>
-    <row r="807" ht="15.75" customHeight="1"/>
-    <row r="808" ht="15.75" customHeight="1"/>
-    <row r="809" ht="15.75" customHeight="1"/>
-    <row r="810" ht="15.75" customHeight="1"/>
-    <row r="811" ht="15.75" customHeight="1"/>
-    <row r="812" ht="15.75" customHeight="1"/>
-    <row r="813" ht="15.75" customHeight="1"/>
-    <row r="814" ht="15.75" customHeight="1"/>
-    <row r="815" ht="15.75" customHeight="1"/>
-    <row r="816" ht="15.75" customHeight="1"/>
-    <row r="817" ht="15.75" customHeight="1"/>
-    <row r="818" ht="15.75" customHeight="1"/>
-    <row r="819" ht="15.75" customHeight="1"/>
-    <row r="820" ht="15.75" customHeight="1"/>
-    <row r="821" ht="15.75" customHeight="1"/>
-    <row r="822" ht="15.75" customHeight="1"/>
-    <row r="823" ht="15.75" customHeight="1"/>
-    <row r="824" ht="15.75" customHeight="1"/>
-    <row r="825" ht="15.75" customHeight="1"/>
-    <row r="826" ht="15.75" customHeight="1"/>
-    <row r="827" ht="15.75" customHeight="1"/>
-    <row r="828" ht="15.75" customHeight="1"/>
-    <row r="829" ht="15.75" customHeight="1"/>
-    <row r="830" ht="15.75" customHeight="1"/>
-    <row r="831" ht="15.75" customHeight="1"/>
-    <row r="832" ht="15.75" customHeight="1"/>
-    <row r="833" ht="15.75" customHeight="1"/>
-    <row r="834" ht="15.75" customHeight="1"/>
-    <row r="835" ht="15.75" customHeight="1"/>
-    <row r="836" ht="15.75" customHeight="1"/>
-    <row r="837" ht="15.75" customHeight="1"/>
-    <row r="838" ht="15.75" customHeight="1"/>
-    <row r="839" ht="15.75" customHeight="1"/>
-    <row r="840" ht="15.75" customHeight="1"/>
-    <row r="841" ht="15.75" customHeight="1"/>
-    <row r="842" ht="15.75" customHeight="1"/>
-    <row r="843" ht="15.75" customHeight="1"/>
-    <row r="844" ht="15.75" customHeight="1"/>
-    <row r="845" ht="15.75" customHeight="1"/>
-    <row r="846" ht="15.75" customHeight="1"/>
-    <row r="847" ht="15.75" customHeight="1"/>
-    <row r="848" ht="15.75" customHeight="1"/>
-    <row r="849" ht="15.75" customHeight="1"/>
-    <row r="850" ht="15.75" customHeight="1"/>
-    <row r="851" ht="15.75" customHeight="1"/>
-    <row r="852" ht="15.75" customHeight="1"/>
-    <row r="853" ht="15.75" customHeight="1"/>
-    <row r="854" ht="15.75" customHeight="1"/>
-    <row r="855" ht="15.75" customHeight="1"/>
-    <row r="856" ht="15.75" customHeight="1"/>
-    <row r="857" ht="15.75" customHeight="1"/>
-    <row r="858" ht="15.75" customHeight="1"/>
-    <row r="859" ht="15.75" customHeight="1"/>
-    <row r="860" ht="15.75" customHeight="1"/>
-    <row r="861" ht="15.75" customHeight="1"/>
-    <row r="862" ht="15.75" customHeight="1"/>
-    <row r="863" ht="15.75" customHeight="1"/>
-    <row r="864" ht="15.75" customHeight="1"/>
-    <row r="865" ht="15.75" customHeight="1"/>
-    <row r="866" ht="15.75" customHeight="1"/>
-    <row r="867" ht="15.75" customHeight="1"/>
-    <row r="868" ht="15.75" customHeight="1"/>
-    <row r="869" ht="15.75" customHeight="1"/>
-    <row r="870" ht="15.75" customHeight="1"/>
-    <row r="871" ht="15.75" customHeight="1"/>
-    <row r="872" ht="15.75" customHeight="1"/>
-    <row r="873" ht="15.75" customHeight="1"/>
-    <row r="874" ht="15.75" customHeight="1"/>
-    <row r="875" ht="15.75" customHeight="1"/>
-    <row r="876" ht="15.75" customHeight="1"/>
-    <row r="877" ht="15.75" customHeight="1"/>
-    <row r="878" ht="15.75" customHeight="1"/>
-    <row r="879" ht="15.75" customHeight="1"/>
-    <row r="880" ht="15.75" customHeight="1"/>
-    <row r="881" ht="15.75" customHeight="1"/>
-    <row r="882" ht="15.75" customHeight="1"/>
-    <row r="883" ht="15.75" customHeight="1"/>
-    <row r="884" ht="15.75" customHeight="1"/>
-    <row r="885" ht="15.75" customHeight="1"/>
-    <row r="886" ht="15.75" customHeight="1"/>
-    <row r="887" ht="15.75" customHeight="1"/>
-    <row r="888" ht="15.75" customHeight="1"/>
-    <row r="889" ht="15.75" customHeight="1"/>
-    <row r="890" ht="15.75" customHeight="1"/>
-    <row r="891" ht="15.75" customHeight="1"/>
-    <row r="892" ht="15.75" customHeight="1"/>
-    <row r="893" ht="15.75" customHeight="1"/>
-    <row r="894" ht="15.75" customHeight="1"/>
-    <row r="895" ht="15.75" customHeight="1"/>
-    <row r="896" ht="15.75" customHeight="1"/>
-    <row r="897" ht="15.75" customHeight="1"/>
-    <row r="898" ht="15.75" customHeight="1"/>
-    <row r="899" ht="15.75" customHeight="1"/>
-    <row r="900" ht="15.75" customHeight="1"/>
-    <row r="901" ht="15.75" customHeight="1"/>
-    <row r="902" ht="15.75" customHeight="1"/>
-    <row r="903" ht="15.75" customHeight="1"/>
-    <row r="904" ht="15.75" customHeight="1"/>
-    <row r="905" ht="15.75" customHeight="1"/>
-    <row r="906" ht="15.75" customHeight="1"/>
-    <row r="907" ht="15.75" customHeight="1"/>
-    <row r="908" ht="15.75" customHeight="1"/>
-    <row r="909" ht="15.75" customHeight="1"/>
-    <row r="910" ht="15.75" customHeight="1"/>
-    <row r="911" ht="15.75" customHeight="1"/>
-    <row r="912" ht="15.75" customHeight="1"/>
-    <row r="913" ht="15.75" customHeight="1"/>
-    <row r="914" ht="15.75" customHeight="1"/>
-    <row r="915" ht="15.75" customHeight="1"/>
-    <row r="916" ht="15.75" customHeight="1"/>
-    <row r="917" ht="15.75" customHeight="1"/>
-    <row r="918" ht="15.75" customHeight="1"/>
-    <row r="919" ht="15.75" customHeight="1"/>
-    <row r="920" ht="15.75" customHeight="1"/>
-    <row r="921" ht="15.75" customHeight="1"/>
-    <row r="922" ht="15.75" customHeight="1"/>
-    <row r="923" ht="15.75" customHeight="1"/>
-    <row r="924" ht="15.75" customHeight="1"/>
-    <row r="925" ht="15.75" customHeight="1"/>
-    <row r="926" ht="15.75" customHeight="1"/>
-    <row r="927" ht="15.75" customHeight="1"/>
-    <row r="928" ht="15.75" customHeight="1"/>
-    <row r="929" ht="15.75" customHeight="1"/>
-    <row r="930" ht="15.75" customHeight="1"/>
-    <row r="931" ht="15.75" customHeight="1"/>
-    <row r="932" ht="15.75" customHeight="1"/>
-    <row r="933" ht="15.75" customHeight="1"/>
-    <row r="934" ht="15.75" customHeight="1"/>
-    <row r="935" ht="15.75" customHeight="1"/>
-    <row r="936" ht="15.75" customHeight="1"/>
-    <row r="937" ht="15.75" customHeight="1"/>
-    <row r="938" ht="15.75" customHeight="1"/>
-    <row r="939" ht="15.75" customHeight="1"/>
-    <row r="940" ht="15.75" customHeight="1"/>
-    <row r="941" ht="15.75" customHeight="1"/>
-    <row r="942" ht="15.75" customHeight="1"/>
-    <row r="943" ht="15.75" customHeight="1"/>
-    <row r="944" ht="15.75" customHeight="1"/>
-    <row r="945" ht="15.75" customHeight="1"/>
-    <row r="946" ht="15.75" customHeight="1"/>
-    <row r="947" ht="15.75" customHeight="1"/>
-    <row r="948" ht="15.75" customHeight="1"/>
-    <row r="949" ht="15.75" customHeight="1"/>
-    <row r="950" ht="15.75" customHeight="1"/>
-    <row r="951" ht="15.75" customHeight="1"/>
-    <row r="952" ht="15.75" customHeight="1"/>
-    <row r="953" ht="15.75" customHeight="1"/>
-    <row r="954" ht="15.75" customHeight="1"/>
-    <row r="955" ht="15.75" customHeight="1"/>
-    <row r="956" ht="15.75" customHeight="1"/>
-    <row r="957" ht="15.75" customHeight="1"/>
-    <row r="958" ht="15.75" customHeight="1"/>
-    <row r="959" ht="15.75" customHeight="1"/>
-    <row r="960" ht="15.75" customHeight="1"/>
-    <row r="961" ht="15.75" customHeight="1"/>
-    <row r="962" ht="15.75" customHeight="1"/>
-    <row r="963" ht="15.75" customHeight="1"/>
-    <row r="964" ht="15.75" customHeight="1"/>
-    <row r="965" ht="15.75" customHeight="1"/>
-    <row r="966" ht="15.75" customHeight="1"/>
-    <row r="967" ht="15.75" customHeight="1"/>
-    <row r="968" ht="15.75" customHeight="1"/>
-    <row r="969" ht="15.75" customHeight="1"/>
-    <row r="970" ht="15.75" customHeight="1"/>
-    <row r="971" ht="15.75" customHeight="1"/>
-    <row r="972" ht="15.75" customHeight="1"/>
-    <row r="973" ht="15.75" customHeight="1"/>
-    <row r="974" ht="15.75" customHeight="1"/>
-    <row r="975" ht="15.75" customHeight="1"/>
-    <row r="976" ht="15.75" customHeight="1"/>
-    <row r="977" ht="15.75" customHeight="1"/>
-    <row r="978" ht="15.75" customHeight="1"/>
-    <row r="979" ht="15.75" customHeight="1"/>
-    <row r="980" ht="15.75" customHeight="1"/>
-    <row r="981" ht="15.75" customHeight="1"/>
-    <row r="982" ht="15.75" customHeight="1"/>
-    <row r="983" ht="15.75" customHeight="1"/>
-    <row r="984" ht="15.75" customHeight="1"/>
-    <row r="985" ht="15.75" customHeight="1"/>
-    <row r="986" ht="15.75" customHeight="1"/>
-    <row r="987" ht="15.75" customHeight="1"/>
-    <row r="988" ht="15.75" customHeight="1"/>
-    <row r="989" ht="15.75" customHeight="1"/>
-    <row r="990" ht="15.75" customHeight="1"/>
-    <row r="991" ht="15.75" customHeight="1"/>
-    <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
-    <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="387" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="388" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="389" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="390" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="391" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="392" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="393" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="394" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="395" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="396" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="397" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="398" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="399" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="400" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="401" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="402" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="403" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="404" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="405" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="406" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="407" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="408" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="409" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="410" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="411" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="412" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="413" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="414" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="415" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="416" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="417" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="418" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="419" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="420" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="421" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="422" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="423" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="424" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="425" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="426" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="427" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="428" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="429" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="430" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="431" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="432" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="433" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="434" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="435" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="436" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="437" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="438" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="439" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="440" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="441" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="442" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="443" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="444" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="445" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="446" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="447" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="448" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="449" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="450" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="451" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="452" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="453" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="454" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="455" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="456" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="457" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="458" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="459" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="460" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="461" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="462" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="463" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="464" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="465" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="473" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="474" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="475" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="478" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="479" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="480" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="481" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="482" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="483" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="484" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="485" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="513" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="514" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="515" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="516" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="517" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="518" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="519" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="520" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="521" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="522" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="523" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="524" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="525" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="526" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="527" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="528" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="529" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="530" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="531" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="532" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="533" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="534" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="535" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="536" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="537" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="538" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="539" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="540" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="541" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="542" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="543" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="544" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="545" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="546" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="547" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="548" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="549" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="550" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="551" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="552" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="553" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="554" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="555" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="556" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="557" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="558" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="559" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="560" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="561" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="562" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="563" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="564" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="565" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="566" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="567" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="568" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="569" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="570" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="571" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="572" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="573" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="574" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="575" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="577" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="578" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="579" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="580" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="581" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="582" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="583" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="584" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="585" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="586" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="587" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="588" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="589" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="590" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="591" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="592" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="593" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="594" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="595" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="596" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="597" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="598" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="599" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="600" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="601" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="602" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="603" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="604" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="605" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="606" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="607" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="608" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="609" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="610" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="611" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="612" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="613" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="614" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="615" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="616" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="617" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="618" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="619" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="620" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="621" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="622" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="623" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="624" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="625" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="626" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="627" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="628" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="629" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="630" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="631" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="632" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="633" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="634" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="635" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="636" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="637" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="638" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="639" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="640" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="641" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="642" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="643" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="644" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="645" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="646" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="647" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="648" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="649" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="650" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="651" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="652" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="653" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="654" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="655" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="656" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="657" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="658" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="659" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="660" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="661" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="662" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="663" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="664" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="665" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="666" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="667" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="668" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="669" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="670" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="671" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="672" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="673" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="674" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="675" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="676" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="677" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="678" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="679" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="680" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="681" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="682" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="683" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="684" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="685" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="686" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="687" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="688" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="689" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="690" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="691" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="692" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="693" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="694" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="695" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="696" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="697" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="698" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="699" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="700" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="701" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="702" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="703" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="704" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="705" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="706" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="707" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="708" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="709" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="710" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="711" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="712" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="713" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="714" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="715" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="716" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="717" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="718" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="719" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="720" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="721" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="722" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="723" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="724" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="725" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="726" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="727" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="728" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="729" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="730" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="731" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="732" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="733" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="734" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="735" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="736" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="737" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="738" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="739" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="740" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="741" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="742" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="743" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="744" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="745" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="746" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="747" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="748" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="749" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="750" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="751" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="752" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="753" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="754" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="755" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="756" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="757" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="758" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="759" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="760" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="761" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="762" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="763" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="764" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="765" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="766" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="767" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="768" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="769" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="770" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="771" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="772" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="773" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="774" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="775" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="776" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="777" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="778" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="779" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="780" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="781" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="782" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="783" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="784" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="785" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="786" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="787" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="788" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="789" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="790" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="791" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="792" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="793" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="794" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="795" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="796" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="797" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="798" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="799" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="800" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="801" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="802" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="803" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="804" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="805" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="806" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="807" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="808" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="809" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="810" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="811" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="812" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="813" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="814" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="815" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="816" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="817" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="818" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="819" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="820" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="821" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="822" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="823" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="824" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="825" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="826" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="827" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="828" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="829" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="830" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="831" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="832" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="833" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="834" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="835" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="836" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="837" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="838" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="839" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="840" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="841" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="842" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="843" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="844" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="845" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="846" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="847" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="848" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="849" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="850" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="851" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="852" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="853" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="854" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="855" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="856" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="857" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="858" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="859" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="860" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="861" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="862" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="863" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="864" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="865" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="866" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="867" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="868" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="869" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="870" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="871" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="872" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="873" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="874" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="875" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="876" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="877" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="878" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="879" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="880" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="881" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="882" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="883" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="884" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="885" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="886" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="887" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="888" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="889" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="890" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="891" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="892" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="893" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="894" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="895" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="896" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="897" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="898" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="899" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="900" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="901" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="902" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="903" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="904" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="905" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="906" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="907" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="908" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="909" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="910" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="911" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="912" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="913" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="914" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="915" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="916" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="917" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="918" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="919" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="920" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="921" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="922" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="923" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="924" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="925" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="926" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="927" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="928" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="929" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="930" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="931" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="932" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="933" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="934" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="935" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="936" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="937" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="938" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="939" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="940" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="941" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="942" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="943" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="944" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="945" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="946" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="947" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="948" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="949" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="950" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="951" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="952" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="953" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="954" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="955" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="956" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="957" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="958" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="959" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="960" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="961" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="962" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="963" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="964" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="965" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="966" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="967" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="968" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="969" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="970" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="971" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="972" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="973" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="974" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="975" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="976" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="977" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="978" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="979" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="980" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="981" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="982" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="983" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="984" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="985" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="986" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="987" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="988" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="989" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="990" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="991" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="992" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="993" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="994" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="995" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="996" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>